<commit_message>
Uploaded new student files
I tweaked the names of some of the student files then updated all student files to match what is in the book. Finally, I re-compiled the book.
</commit_message>
<xml_diff>
--- a/Student Files/CH3-Data.xlsx
+++ b/Student Files/CH3-Data.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23001"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Excel OER\Chapter3\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gself\Desktop\Excel 365 Exercises\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9AE9053-26B7-4579-991B-FB382FAF54A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7980"/>
+    <workbookView xWindow="1170" yWindow="1170" windowWidth="19365" windowHeight="14205" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Grades" sheetId="2" r:id="rId1"/>
@@ -170,9 +171,9 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
+    <numFmt numFmtId="164" formatCode="[$-409]m/d/yy\ h:mm\ AM/PM;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -259,7 +260,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -296,9 +297,10 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -578,30 +580,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:R2"/>
+      <selection activeCell="O25" sqref="O25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19" style="2" customWidth="1"/>
-    <col min="2" max="4" width="4.77734375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="6.77734375" style="2" customWidth="1"/>
-    <col min="6" max="8" width="4.77734375" style="2" customWidth="1"/>
-    <col min="9" max="9" width="6.77734375" style="2" customWidth="1"/>
-    <col min="10" max="12" width="4.77734375" style="2" customWidth="1"/>
-    <col min="13" max="13" width="6.77734375" style="2" customWidth="1"/>
-    <col min="14" max="14" width="8.5546875" style="2" customWidth="1"/>
-    <col min="15" max="15" width="8.77734375" style="2" customWidth="1"/>
-    <col min="16" max="17" width="11.109375" style="2" customWidth="1"/>
-    <col min="18" max="18" width="6.77734375" style="2" customWidth="1"/>
-    <col min="19" max="16384" width="8.88671875" style="2"/>
+    <col min="2" max="4" width="4.7109375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" style="2" customWidth="1"/>
+    <col min="6" max="8" width="4.7109375" style="2" customWidth="1"/>
+    <col min="9" max="9" width="6.7109375" style="2" customWidth="1"/>
+    <col min="10" max="12" width="4.7109375" style="2" customWidth="1"/>
+    <col min="13" max="13" width="6.7109375" style="2" customWidth="1"/>
+    <col min="14" max="14" width="8.5703125" style="2" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" style="2" customWidth="1"/>
+    <col min="16" max="16" width="12" style="2" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.140625" style="2" customWidth="1"/>
+    <col min="18" max="18" width="6.7109375" style="2" customWidth="1"/>
+    <col min="19" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="19" t="s">
         <v>45</v>
       </c>
@@ -623,7 +626,7 @@
       <c r="Q1" s="19"/>
       <c r="R1" s="19"/>
     </row>
-    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:18" ht="21" x14ac:dyDescent="0.35">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="20"/>
@@ -643,7 +646,7 @@
       <c r="Q2" s="20"/>
       <c r="R2" s="20"/>
     </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A3" s="18"/>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -663,7 +666,7 @@
       <c r="Q3" s="18"/>
       <c r="R3" s="18"/>
     </row>
-    <row r="4" spans="1:18" ht="31.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:18" ht="63" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>0</v>
       </c>
@@ -719,7 +722,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A5" s="12" t="s">
         <v>27</v>
       </c>
@@ -767,7 +770,7 @@
       <c r="Q5"/>
       <c r="R5"/>
     </row>
-    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A6" s="12" t="s">
         <v>30</v>
       </c>
@@ -815,7 +818,7 @@
       <c r="Q6"/>
       <c r="R6"/>
     </row>
-    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A7" s="12" t="s">
         <v>31</v>
       </c>
@@ -863,7 +866,7 @@
       <c r="Q7"/>
       <c r="R7"/>
     </row>
-    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A8" s="12" t="s">
         <v>32</v>
       </c>
@@ -911,7 +914,7 @@
       <c r="Q8"/>
       <c r="R8"/>
     </row>
-    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A9" s="12" t="s">
         <v>29</v>
       </c>
@@ -959,7 +962,7 @@
       <c r="Q9"/>
       <c r="R9"/>
     </row>
-    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A10" s="12" t="s">
         <v>26</v>
       </c>
@@ -1007,7 +1010,7 @@
       <c r="Q10"/>
       <c r="R10"/>
     </row>
-    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A11" s="12" t="s">
         <v>18</v>
       </c>
@@ -1055,7 +1058,7 @@
       <c r="Q11"/>
       <c r="R11"/>
     </row>
-    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>19</v>
       </c>
@@ -1103,7 +1106,7 @@
       <c r="Q12"/>
       <c r="R12"/>
     </row>
-    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A13" s="12" t="s">
         <v>16</v>
       </c>
@@ -1151,7 +1154,7 @@
       <c r="Q13"/>
       <c r="R13"/>
     </row>
-    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A14" s="12" t="s">
         <v>25</v>
       </c>
@@ -1199,7 +1202,7 @@
       <c r="Q14"/>
       <c r="R14"/>
     </row>
-    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A15" s="12" t="s">
         <v>23</v>
       </c>
@@ -1247,7 +1250,7 @@
       <c r="Q15"/>
       <c r="R15"/>
     </row>
-    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A16" s="12" t="s">
         <v>33</v>
       </c>
@@ -1295,7 +1298,7 @@
       <c r="Q16"/>
       <c r="R16"/>
     </row>
-    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A17" s="12" t="s">
         <v>22</v>
       </c>
@@ -1343,7 +1346,7 @@
       <c r="Q17"/>
       <c r="R17"/>
     </row>
-    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A18" s="12" t="s">
         <v>35</v>
       </c>
@@ -1391,7 +1394,7 @@
       <c r="Q18"/>
       <c r="R18"/>
     </row>
-    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A19" s="12" t="s">
         <v>24</v>
       </c>
@@ -1439,7 +1442,7 @@
       <c r="Q19"/>
       <c r="R19"/>
     </row>
-    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A20" s="12" t="s">
         <v>20</v>
       </c>
@@ -1487,7 +1490,7 @@
       <c r="Q20"/>
       <c r="R20"/>
     </row>
-    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A21" s="12" t="s">
         <v>28</v>
       </c>
@@ -1535,7 +1538,7 @@
       <c r="Q21"/>
       <c r="R21"/>
     </row>
-    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
         <v>21</v>
       </c>
@@ -1583,7 +1586,7 @@
       <c r="Q22"/>
       <c r="R22"/>
     </row>
-    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A23" s="12" t="s">
         <v>34</v>
       </c>
@@ -1631,7 +1634,7 @@
       <c r="Q23"/>
       <c r="R23"/>
     </row>
-    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A24" s="12" t="s">
         <v>17</v>
       </c>
@@ -1679,7 +1682,7 @@
       <c r="Q24"/>
       <c r="R24"/>
     </row>
-    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
         <v>15</v>
       </c>
@@ -1696,20 +1699,20 @@
       <c r="L25" s="4"/>
       <c r="M25" s="10"/>
       <c r="N25" s="4"/>
-      <c r="O25" s="1"/>
+      <c r="O25" s="21"/>
       <c r="P25" s="1"/>
       <c r="Q25" s="1"/>
       <c r="R25" s="1"/>
     </row>
-    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:18" x14ac:dyDescent="0.25">
       <c r="I26" s="11"/>
     </row>
-    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A28" s="5">
         <v>0</v>
       </c>
@@ -1717,7 +1720,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>0.6</v>
       </c>
@@ -1725,7 +1728,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
         <v>0.7</v>
       </c>
@@ -1733,7 +1736,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A31" s="5">
         <v>0.8</v>
       </c>
@@ -1741,7 +1744,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A32" s="5">
         <v>0.9</v>
       </c>

</xml_diff>